<commit_message>
Updating all code and documentation files.
</commit_message>
<xml_diff>
--- a/data/identifiers_match.xlsx
+++ b/data/identifiers_match.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\github\MAGENTA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38251C09-0DF8-4621-85B0-C59A66DD3CE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C637E33-1EA7-4E52-813D-AE02E79A6AF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="70" windowWidth="19200" windowHeight="10730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,9 +45,6 @@
     <t>CHL</t>
   </si>
   <si>
-    <t>CHLORAMPHENICOL-1.5 - UNSPECIFIED</t>
-  </si>
-  <si>
     <t>CIP</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>RIF</t>
   </si>
   <si>
-    <t>RIFAMPICIN-1.0 - UNSPECIFIED</t>
-  </si>
-  <si>
     <t>TET</t>
   </si>
   <si>
@@ -144,10 +138,16 @@
     <t>SPE</t>
   </si>
   <si>
-    <t>SPECTINOMYCIN-4.0 - UNSPECIFIED</t>
-  </si>
-  <si>
     <t>CIPROFLOXACIN-0.008 - UNSPECIFIED</t>
+  </si>
+  <si>
+    <t>CHLORAMPHENICOL-2.0- UNSPECIFIED</t>
+  </si>
+  <si>
+    <t>RIFAMPICIN-2.0 - UNSPECIFIED</t>
+  </si>
+  <si>
+    <t>SPECTINOMYCIN-6.0 - UNSPECIFIED</t>
   </si>
 </sst>
 </file>
@@ -468,7 +468,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -486,143 +486,143 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
         <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
         <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
         <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
         <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>